<commit_message>
Removed silverlight apps, prism library, silverlight modules, extjs 3 also removed joseki related projects added extjs 4 minimum requirements
</commit_message>
<xml_diff>
--- a/Documentation/iRINGTools_Dev_Test_Plan_v2.1.0.xlsx
+++ b/Documentation/iRINGTools_Dev_Test_Plan_v2.1.0.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="16275" windowHeight="11310"/>
@@ -12,12 +12,12 @@
     <sheet name="Specialized Templates" sheetId="3" r:id="rId3"/>
     <sheet name="OracleDatabase" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="33">
   <si>
     <t>Search</t>
   </si>
@@ -84,12 +84,45 @@
   <si>
     <t>Verify Edit</t>
   </si>
+  <si>
+    <t>Class Added to local repo</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Further notes are Part8 Classes do have the following properties</t>
+  </si>
+  <si>
+    <t>Added by selecting from other repo and save to local repo</t>
+  </si>
+  <si>
+    <t>3) must have rdfs:label</t>
+  </si>
+  <si>
+    <t>4) optional rdfs:comment</t>
+  </si>
+  <si>
+    <t>1) is rdf:type owl:Class</t>
+  </si>
+  <si>
+    <t>2) is rdf:type dm:{class}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5) optional are rdfs:subClassOf superclasse(s)  </t>
+  </si>
+  <si>
+    <t>6) optional have rdfs:subClassOf subclasse(s)</t>
+  </si>
+  <si>
+    <t>STRAIGHT LINEAR DISTANCE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +137,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF30332D"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -126,13 +165,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -224,7 +275,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -259,7 +309,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -435,24 +484,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFC12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:XFC14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16383">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -16853,18 +16904,36 @@
       <c r="XFB1" s="2"/>
       <c r="XFC1" s="2"/>
     </row>
-    <row r="2" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16383" ht="63.75" customHeight="1">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16383">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -16875,8 +16944,16 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
+      <c r="H3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16383">
       <c r="A4">
         <f t="shared" ref="A4:A12" si="0">A3+1</f>
         <v>3</v>
@@ -16887,8 +16964,16 @@
       <c r="C4" t="s">
         <v>0</v>
       </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16383">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -16899,8 +16984,16 @@
       <c r="C5" t="s">
         <v>1</v>
       </c>
+      <c r="H5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16383">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -16911,8 +17004,16 @@
       <c r="C6" t="s">
         <v>2</v>
       </c>
+      <c r="H6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16383">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -16923,8 +17024,16 @@
       <c r="C7" t="s">
         <v>7</v>
       </c>
+      <c r="H7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16383">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -16935,8 +17044,16 @@
       <c r="C8" t="s">
         <v>8</v>
       </c>
+      <c r="H8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16383">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -16947,8 +17064,16 @@
       <c r="C9" t="s">
         <v>9</v>
       </c>
+      <c r="H9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
     </row>
-    <row r="10" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16383">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -16959,8 +17084,14 @@
       <c r="C10" t="s">
         <v>10</v>
       </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16383">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -16971,8 +17102,14 @@
       <c r="C11" t="s">
         <v>6</v>
       </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16383">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -16983,24 +17120,47 @@
       <c r="C12" t="s">
         <v>4</v>
       </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="1:16383">
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+    </row>
+    <row r="14" spans="1:16383">
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="192" verticalDpi="192" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -17009,7 +17169,7 @@
     <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="30">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -17035,7 +17195,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -17046,7 +17206,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -17058,7 +17218,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4">
         <f t="shared" ref="A4:A12" si="0">A3+1</f>
         <v>3</v>
@@ -17070,7 +17230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -17082,7 +17242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -17094,7 +17254,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -17106,7 +17266,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -17118,7 +17278,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -17130,7 +17290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -17142,7 +17302,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -17154,7 +17314,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -17172,20 +17332,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="30">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -17211,7 +17372,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -17222,7 +17383,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -17234,7 +17395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4">
         <f t="shared" ref="A4:A12" si="0">A3+1</f>
         <v>3</v>
@@ -17246,7 +17407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -17258,7 +17419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -17270,7 +17431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -17282,7 +17443,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -17294,7 +17455,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -17306,7 +17467,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -17318,7 +17479,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -17330,7 +17491,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -17348,14 +17509,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Need to back port features from trunk to support new DL features.
</commit_message>
<xml_diff>
--- a/Documentation/iRINGTools_Dev_Test_Plan_v2.1.0.xlsx
+++ b/Documentation/iRINGTools_Dev_Test_Plan_v2.1.0.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="16275" windowHeight="11310"/>
@@ -12,12 +12,12 @@
     <sheet name="Specialized Templates" sheetId="3" r:id="rId3"/>
     <sheet name="OracleDatabase" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="22">
   <si>
     <t>Search</t>
   </si>
@@ -84,45 +84,12 @@
   <si>
     <t>Verify Edit</t>
   </si>
-  <si>
-    <t>Class Added to local repo</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Further notes are Part8 Classes do have the following properties</t>
-  </si>
-  <si>
-    <t>Added by selecting from other repo and save to local repo</t>
-  </si>
-  <si>
-    <t>3) must have rdfs:label</t>
-  </si>
-  <si>
-    <t>4) optional rdfs:comment</t>
-  </si>
-  <si>
-    <t>1) is rdf:type owl:Class</t>
-  </si>
-  <si>
-    <t>2) is rdf:type dm:{class}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5) optional are rdfs:subClassOf superclasse(s)  </t>
-  </si>
-  <si>
-    <t>6) optional have rdfs:subClassOf subclasse(s)</t>
-  </si>
-  <si>
-    <t>STRAIGHT LINEAR DISTANCE</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,12 +104,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF30332D"/>
-      <name val="Courier New"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -165,25 +126,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -275,6 +224,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -309,6 +259,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -484,26 +435,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFC14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:XFC12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16383">
+    <row r="1" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -16904,36 +16853,18 @@
       <c r="XFB1" s="2"/>
       <c r="XFC1" s="2"/>
     </row>
-    <row r="2" spans="1:16383" ht="63.75" customHeight="1">
+    <row r="2" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:16383">
+    <row r="3" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -16944,16 +16875,8 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:16383">
+    <row r="4" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A12" si="0">A3+1</f>
         <v>3</v>
@@ -16964,16 +16887,8 @@
       <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="H4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="1:16383">
+    <row r="5" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -16984,16 +16899,8 @@
       <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="1:16383">
+    <row r="6" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -17004,16 +16911,8 @@
       <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:16383">
+    <row r="7" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -17024,16 +16923,8 @@
       <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="1:16383">
+    <row r="8" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -17044,16 +16935,8 @@
       <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="1:16383">
+    <row r="9" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -17064,16 +16947,8 @@
       <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
     </row>
-    <row r="10" spans="1:16383">
+    <row r="10" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -17084,14 +16959,8 @@
       <c r="C10" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="1:16383">
+    <row r="11" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -17102,14 +16971,8 @@
       <c r="C11" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="1:16383">
+    <row r="12" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -17120,47 +16983,24 @@
       <c r="C12" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-    </row>
-    <row r="13" spans="1:16383">
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-    </row>
-    <row r="14" spans="1:16383">
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="192" verticalDpi="192" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -17169,7 +17009,7 @@
     <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -17195,7 +17035,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -17206,7 +17046,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -17218,7 +17058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A12" si="0">A3+1</f>
         <v>3</v>
@@ -17230,7 +17070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -17242,7 +17082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -17254,7 +17094,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -17266,7 +17106,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -17278,7 +17118,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -17290,7 +17130,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -17302,7 +17142,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -17314,7 +17154,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -17332,21 +17172,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -17372,7 +17211,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -17383,7 +17222,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -17395,7 +17234,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A12" si="0">A3+1</f>
         <v>3</v>
@@ -17407,7 +17246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -17419,7 +17258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -17431,7 +17270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -17443,7 +17282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -17455,7 +17294,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -17467,7 +17306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -17479,7 +17318,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -17491,7 +17330,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -17509,14 +17348,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Stable 2.4 build (431) from bamboo
</commit_message>
<xml_diff>
--- a/Documentation/iRINGTools_Dev_Test_Plan_v2.1.0.xlsx
+++ b/Documentation/iRINGTools_Dev_Test_Plan_v2.1.0.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="16275" windowHeight="11310"/>
@@ -12,12 +12,12 @@
     <sheet name="Specialized Templates" sheetId="3" r:id="rId3"/>
     <sheet name="OracleDatabase" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="22">
   <si>
     <t>Search</t>
   </si>
@@ -84,45 +84,12 @@
   <si>
     <t>Verify Edit</t>
   </si>
-  <si>
-    <t>Class Added to local repo</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Further notes are Part8 Classes do have the following properties</t>
-  </si>
-  <si>
-    <t>Added by selecting from other repo and save to local repo</t>
-  </si>
-  <si>
-    <t>3) must have rdfs:label</t>
-  </si>
-  <si>
-    <t>4) optional rdfs:comment</t>
-  </si>
-  <si>
-    <t>1) is rdf:type owl:Class</t>
-  </si>
-  <si>
-    <t>2) is rdf:type dm:{class}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5) optional are rdfs:subClassOf superclasse(s)  </t>
-  </si>
-  <si>
-    <t>6) optional have rdfs:subClassOf subclasse(s)</t>
-  </si>
-  <si>
-    <t>STRAIGHT LINEAR DISTANCE</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,12 +104,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF30332D"/>
-      <name val="Courier New"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -165,25 +126,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -275,6 +224,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -309,6 +259,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -484,26 +435,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFC14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:XFC12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16383">
+    <row r="1" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -16904,36 +16853,18 @@
       <c r="XFB1" s="2"/>
       <c r="XFC1" s="2"/>
     </row>
-    <row r="2" spans="1:16383" ht="63.75" customHeight="1">
+    <row r="2" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:16383">
+    <row r="3" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -16944,16 +16875,8 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:16383">
+    <row r="4" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A12" si="0">A3+1</f>
         <v>3</v>
@@ -16964,16 +16887,8 @@
       <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="H4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="1:16383">
+    <row r="5" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -16984,16 +16899,8 @@
       <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="1:16383">
+    <row r="6" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -17004,16 +16911,8 @@
       <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:16383">
+    <row r="7" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -17024,16 +16923,8 @@
       <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="1:16383">
+    <row r="8" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -17044,16 +16935,8 @@
       <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="1:16383">
+    <row r="9" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -17064,16 +16947,8 @@
       <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
     </row>
-    <row r="10" spans="1:16383">
+    <row r="10" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -17084,14 +16959,8 @@
       <c r="C10" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="1:16383">
+    <row r="11" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -17102,14 +16971,8 @@
       <c r="C11" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="1:16383">
+    <row r="12" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -17120,47 +16983,24 @@
       <c r="C12" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-    </row>
-    <row r="13" spans="1:16383">
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-    </row>
-    <row r="14" spans="1:16383">
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="192" verticalDpi="192" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -17169,7 +17009,7 @@
     <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -17195,7 +17035,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -17206,7 +17046,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -17218,7 +17058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A12" si="0">A3+1</f>
         <v>3</v>
@@ -17230,7 +17070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -17242,7 +17082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -17254,7 +17094,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -17266,7 +17106,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -17278,7 +17118,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -17290,7 +17130,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -17302,7 +17142,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -17314,7 +17154,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -17332,21 +17172,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -17372,7 +17211,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -17383,7 +17222,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -17395,7 +17234,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A12" si="0">A3+1</f>
         <v>3</v>
@@ -17407,7 +17246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -17419,7 +17258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -17431,7 +17270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -17443,7 +17282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -17455,7 +17294,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -17467,7 +17306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -17479,7 +17318,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -17491,7 +17330,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -17509,14 +17348,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
before internal data layer implementation
</commit_message>
<xml_diff>
--- a/Documentation/iRINGTools_Dev_Test_Plan_v2.1.0.xlsx
+++ b/Documentation/iRINGTools_Dev_Test_Plan_v2.1.0.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="16275" windowHeight="11310"/>
@@ -12,12 +12,12 @@
     <sheet name="Specialized Templates" sheetId="3" r:id="rId3"/>
     <sheet name="OracleDatabase" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="22">
   <si>
     <t>Search</t>
   </si>
@@ -84,45 +84,12 @@
   <si>
     <t>Verify Edit</t>
   </si>
-  <si>
-    <t>Class Added to local repo</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Further notes are Part8 Classes do have the following properties</t>
-  </si>
-  <si>
-    <t>Added by selecting from other repo and save to local repo</t>
-  </si>
-  <si>
-    <t>3) must have rdfs:label</t>
-  </si>
-  <si>
-    <t>4) optional rdfs:comment</t>
-  </si>
-  <si>
-    <t>1) is rdf:type owl:Class</t>
-  </si>
-  <si>
-    <t>2) is rdf:type dm:{class}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5) optional are rdfs:subClassOf superclasse(s)  </t>
-  </si>
-  <si>
-    <t>6) optional have rdfs:subClassOf subclasse(s)</t>
-  </si>
-  <si>
-    <t>STRAIGHT LINEAR DISTANCE</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,12 +104,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF30332D"/>
-      <name val="Courier New"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -165,25 +126,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -275,6 +224,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -309,6 +259,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -484,26 +435,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFC14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:XFC12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16383">
+    <row r="1" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -16904,36 +16853,18 @@
       <c r="XFB1" s="2"/>
       <c r="XFC1" s="2"/>
     </row>
-    <row r="2" spans="1:16383" ht="63.75" customHeight="1">
+    <row r="2" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:16383">
+    <row r="3" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -16944,16 +16875,8 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:16383">
+    <row r="4" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A12" si="0">A3+1</f>
         <v>3</v>
@@ -16964,16 +16887,8 @@
       <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="H4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="1:16383">
+    <row r="5" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -16984,16 +16899,8 @@
       <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="1:16383">
+    <row r="6" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -17004,16 +16911,8 @@
       <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:16383">
+    <row r="7" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -17024,16 +16923,8 @@
       <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="1:16383">
+    <row r="8" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -17044,16 +16935,8 @@
       <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="1:16383">
+    <row r="9" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -17064,16 +16947,8 @@
       <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
     </row>
-    <row r="10" spans="1:16383">
+    <row r="10" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -17084,14 +16959,8 @@
       <c r="C10" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="1:16383">
+    <row r="11" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -17102,14 +16971,8 @@
       <c r="C11" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="1:16383">
+    <row r="12" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -17120,47 +16983,24 @@
       <c r="C12" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-    </row>
-    <row r="13" spans="1:16383">
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-    </row>
-    <row r="14" spans="1:16383">
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="192" verticalDpi="192" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -17169,7 +17009,7 @@
     <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -17195,7 +17035,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -17206,7 +17046,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -17218,7 +17058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A12" si="0">A3+1</f>
         <v>3</v>
@@ -17230,7 +17070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -17242,7 +17082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -17254,7 +17094,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -17266,7 +17106,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -17278,7 +17118,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -17290,7 +17130,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -17302,7 +17142,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -17314,7 +17154,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -17332,21 +17172,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -17372,7 +17211,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -17383,7 +17222,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -17395,7 +17234,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A12" si="0">A3+1</f>
         <v>3</v>
@@ -17407,7 +17246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -17419,7 +17258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -17431,7 +17270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -17443,7 +17282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -17455,7 +17294,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -17467,7 +17306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -17479,7 +17318,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -17491,7 +17330,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -17509,14 +17348,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>